<commit_message>
remove dhs_religion_ethnicity.ado and include in dhs_read.ado
</commit_message>
<xml_diff>
--- a/auxiliary_data/filenames.xlsx
+++ b/auxiliary_data/filenames.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="dhs_pr_files" sheetId="1" state="visible" r:id="rId2"/>
@@ -3411,12 +3411,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -3428,15 +3428,15 @@
   </sheetPr>
   <dimension ref="A1:D173"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.24609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5864,10 +5864,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5879,16 +5879,14 @@
   </sheetPr>
   <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.24609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8106,10 +8104,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -8121,13 +8119,15 @@
   </sheetPr>
   <dimension ref="A1:D133"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.24609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="25.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9995,10 +9995,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -10010,16 +10010,14 @@
   </sheetPr>
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.24609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11033,10 +11031,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update README and fix bugs
</commit_message>
<xml_diff>
--- a/auxiliary_data/filenames.xlsx
+++ b/auxiliary_data/filenames.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dhs_pr_files" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="1101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="1093">
   <si>
     <t xml:space="preserve">folder_country</t>
   </si>
@@ -745,10 +745,10 @@
     <t xml:space="preserve">Maldives</t>
   </si>
   <si>
-    <t xml:space="preserve">MVPR51FL.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maldives/2009/MVPR51FL.dta</t>
+    <t xml:space="preserve">MVPR52FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maldives/2009/MVPR52FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">MVPR71FL.dta</t>
@@ -871,10 +871,10 @@
     <t xml:space="preserve">Namibia/2006/NMPR52FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">NMPR60FL.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namibia/2013/NMPR60FL.dta</t>
+    <t xml:space="preserve">NMPR61FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namibia/2013/NMPR61FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">Nepal</t>
@@ -985,16 +985,16 @@
     <t xml:space="preserve">Turkey</t>
   </si>
   <si>
-    <t xml:space="preserve">RESHAPE_trhr50fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turkey/2008/RESHAPE_trhr50fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESHAPE_trhr61fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turkey/2013/RESHAPE_trhr61fl.dta</t>
+    <t xml:space="preserve">TRHR50FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey/2008/TRHR50FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRHR61FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey/2013/TRHR61FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda</t>
@@ -1381,7 +1381,7 @@
     <t xml:space="preserve">BJIR71FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">Benin/2017/BJIR71FL.dta</t>
+    <t xml:space="preserve">Benin/2018/BJIR71FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">BOIR41FL.dta</t>
@@ -1642,10 +1642,10 @@
     <t xml:space="preserve">Guinea/1999/GNIR41FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">gnir52fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guinea/2005/gnir52fl.dta</t>
+    <t xml:space="preserve">GNIR52FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guinea/2005/GNIR52FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">GNIR61FL.dta</t>
@@ -1696,12 +1696,6 @@
     <t xml:space="preserve">India/2005/IAIR52FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">IAIR74FL.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">India/2015/IAIR74FL.dta</t>
-  </si>
-  <si>
     <t xml:space="preserve">IDIR42FL.dta</t>
   </si>
   <si>
@@ -1834,10 +1828,10 @@
     <t xml:space="preserve">Malawi/2015/MWIR7HFL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">MVIR51FL.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maldives/2009/MVIR51FL.dta</t>
+    <t xml:space="preserve">MVIR52FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maldives/2009/MVIR52FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">MLIR41FL.dta</t>
@@ -1888,16 +1882,16 @@
     <t xml:space="preserve">Namibia/2000/NMIR41FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">nmir51fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namibia/2006/nmir51fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMIR60FL.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namibia/2013/NMIR60FL.dta</t>
+    <t xml:space="preserve">NMIR51FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namibia/2006/NMIR51FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMIR61FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namibia/2013/NMIR61FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">NPIR41FL.dta</t>
@@ -1918,12 +1912,6 @@
     <t xml:space="preserve">Nepal/2011/NPIR60FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">NPIR7HFL.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nepal/2016/NPIR7HFL.dta</t>
-  </si>
-  <si>
     <t xml:space="preserve">NCIR41FL.dta</t>
   </si>
   <si>
@@ -1972,10 +1960,10 @@
     <t xml:space="preserve">Nigeria/2018/NGIR7AFL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">pkir52fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pakistan/2006/pkir52fl.dta</t>
+    <t xml:space="preserve">PKIR52FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pakistan/2006/PKIR52FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">PKIR61FL.dta</t>
@@ -2092,10 +2080,10 @@
     <t xml:space="preserve">SierraLeone/2013/SLIR61FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">szir51fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swaziland/2006/szir51fl.dta</t>
+    <t xml:space="preserve">SZIR51FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swaziland/2006/SZIR51FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">TJIR61FL.dta</t>
@@ -2317,7 +2305,7 @@
     <t xml:space="preserve">BJMR71FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">Benin/2017/BJMR71FL.dta</t>
+    <t xml:space="preserve">Benin/2018/BJMR71FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">BOMR41FL.dta</t>
@@ -2530,10 +2518,10 @@
     <t xml:space="preserve">Guinea/1999/GNMR41FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">gnMR52fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guinea/2005/gnMR52fl.dta</t>
+    <t xml:space="preserve">GNMR52FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guinea/2005/GNMR52FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">GNMR61FL.dta</t>
@@ -2578,12 +2566,6 @@
     <t xml:space="preserve">India/2005/IAMR52FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">IAMR74FL.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">India/2015/IAMR74FL.dta</t>
-  </si>
-  <si>
     <t xml:space="preserve">IDMR42FL.dta</t>
   </si>
   <si>
@@ -2698,10 +2680,10 @@
     <t xml:space="preserve">Malawi/2015/MWMR7HFL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">MVMR51FL.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maldives/2009/MVMR51FL.dta</t>
+    <t xml:space="preserve">MVMR52FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maldives/2009/MVMR52FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">MLMR41FL.dta</t>
@@ -2746,16 +2728,16 @@
     <t xml:space="preserve">Namibia/2000/NMMR41FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">nmMR51fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namibia/2006/nmMR51fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMMR60FL.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namibia/2013/NMMR60FL.dta</t>
+    <t xml:space="preserve">NMMR51FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namibia/2006/NMMR51FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMMR61FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namibia/2013/NMMR61FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">NPMR41FL.dta</t>
@@ -2908,10 +2890,10 @@
     <t xml:space="preserve">SierraLeone/2013/SLMR61FL.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">szMR51fl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swaziland/2006/szMR51fl.dta</t>
+    <t xml:space="preserve">SZMR51FL.dta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swaziland/2006/SZMR51FL.dta</t>
   </si>
   <si>
     <t xml:space="preserve">TLMR61FL.dta</t>
@@ -3079,9 +3061,6 @@
     <t xml:space="preserve">Chad/2010/hl.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">Congo/2015/hl.dta</t>
-  </si>
-  <si>
     <t xml:space="preserve">CostaRica</t>
   </si>
   <si>
@@ -3113,9 +3092,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ghana/2011/hl.dta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guinea/2016/hl.dta</t>
   </si>
   <si>
     <t xml:space="preserve">Guinea-Bissau</t>
@@ -3411,12 +3387,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -3428,15 +3404,17 @@
   </sheetPr>
   <dimension ref="A1:D173"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.24609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.63"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="65.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5864,10 +5842,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5877,16 +5855,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D158"/>
+  <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.24609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.18"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.9540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6132,7 +6113,7 @@
         <v>43</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>451</v>
@@ -6871,10 +6852,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>2015</v>
+        <v>2002</v>
       </c>
       <c r="C71" s="0" t="s">
         <v>557</v>
@@ -6888,7 +6869,7 @@
         <v>163</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>2002</v>
+        <v>2007</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>559</v>
@@ -6902,7 +6883,7 @@
         <v>163</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>2007</v>
+        <v>2012</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>561</v>
@@ -6913,10 +6894,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>2012</v>
+        <v>2002</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>563</v>
@@ -6930,7 +6911,7 @@
         <v>172</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>2002</v>
+        <v>2007</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>565</v>
@@ -6944,7 +6925,7 @@
         <v>172</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>2007</v>
+        <v>2012</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>567</v>
@@ -6955,10 +6936,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>172</v>
+        <v>195</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>2012</v>
+        <v>1999</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>569</v>
@@ -6969,10 +6950,10 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>1999</v>
+        <v>2003</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>571</v>
@@ -6986,7 +6967,7 @@
         <v>179</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>2003</v>
+        <v>2008</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>573</v>
@@ -7000,7 +6981,7 @@
         <v>179</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>575</v>
@@ -7011,10 +6992,10 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>577</v>
@@ -7025,10 +7006,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>2012</v>
+        <v>2004</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>579</v>
@@ -7042,7 +7023,7 @@
         <v>209</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>2004</v>
+        <v>2009</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>581</v>
@@ -7056,7 +7037,7 @@
         <v>209</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>2009</v>
+        <v>2014</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>583</v>
@@ -7067,10 +7048,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>585</v>
@@ -7084,7 +7065,7 @@
         <v>204</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="C86" s="0" t="s">
         <v>587</v>
@@ -7095,10 +7076,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>2013</v>
+        <v>2003</v>
       </c>
       <c r="C87" s="0" t="s">
         <v>589</v>
@@ -7112,7 +7093,7 @@
         <v>222</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>2003</v>
+        <v>2008</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>591</v>
@@ -7123,10 +7104,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>593</v>
@@ -7140,7 +7121,7 @@
         <v>244</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>2000</v>
+        <v>2004</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>595</v>
@@ -7154,7 +7135,7 @@
         <v>244</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>2004</v>
+        <v>2010</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>597</v>
@@ -7168,7 +7149,7 @@
         <v>244</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>599</v>
@@ -7179,10 +7160,10 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>601</v>
@@ -7193,10 +7174,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>2009</v>
+        <v>2001</v>
       </c>
       <c r="C94" s="0" t="s">
         <v>603</v>
@@ -7210,7 +7191,7 @@
         <v>227</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>2001</v>
+        <v>2006</v>
       </c>
       <c r="C95" s="0" t="s">
         <v>605</v>
@@ -7224,7 +7205,7 @@
         <v>227</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="C96" s="0" t="s">
         <v>607</v>
@@ -7235,10 +7216,10 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>609</v>
@@ -7249,7 +7230,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>216</v>
+        <v>253</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>2003</v>
@@ -7266,7 +7247,7 @@
         <v>253</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>2003</v>
+        <v>2011</v>
       </c>
       <c r="C99" s="0" t="s">
         <v>613</v>
@@ -7277,10 +7258,10 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="C100" s="0" t="s">
         <v>615</v>
@@ -7291,10 +7272,10 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>236</v>
+        <v>277</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="C101" s="0" t="s">
         <v>617</v>
@@ -7308,7 +7289,7 @@
         <v>277</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="C102" s="0" t="s">
         <v>619</v>
@@ -7322,7 +7303,7 @@
         <v>277</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>2006</v>
+        <v>2013</v>
       </c>
       <c r="C103" s="0" t="s">
         <v>621</v>
@@ -7333,10 +7314,10 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>2013</v>
+        <v>2001</v>
       </c>
       <c r="C104" s="0" t="s">
         <v>623</v>
@@ -7350,7 +7331,7 @@
         <v>284</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>2001</v>
+        <v>2006</v>
       </c>
       <c r="C105" s="0" t="s">
         <v>625</v>
@@ -7364,7 +7345,7 @@
         <v>284</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="C106" s="0" t="s">
         <v>627</v>
@@ -7375,10 +7356,10 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>2011</v>
+        <v>2001</v>
       </c>
       <c r="C107" s="0" t="s">
         <v>629</v>
@@ -7389,10 +7370,10 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>2016</v>
+        <v>2006</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>631</v>
@@ -7403,10 +7384,10 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>2001</v>
+        <v>2012</v>
       </c>
       <c r="C109" s="0" t="s">
         <v>633</v>
@@ -7417,10 +7398,10 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>2006</v>
+        <v>1999</v>
       </c>
       <c r="C110" s="0" t="s">
         <v>635</v>
@@ -7431,10 +7412,10 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="C111" s="0" t="s">
         <v>637</v>
@@ -7448,7 +7429,7 @@
         <v>261</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>1999</v>
+        <v>2008</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>639</v>
@@ -7462,7 +7443,7 @@
         <v>261</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>2003</v>
+        <v>2013</v>
       </c>
       <c r="C113" s="0" t="s">
         <v>641</v>
@@ -7476,7 +7457,7 @@
         <v>261</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>643</v>
@@ -7487,10 +7468,10 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>261</v>
+        <v>312</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="C115" s="0" t="s">
         <v>645</v>
@@ -7501,10 +7482,10 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>261</v>
+        <v>312</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="C116" s="0" t="s">
         <v>647</v>
@@ -7515,10 +7496,10 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="C117" s="0" t="s">
         <v>649</v>
@@ -7529,10 +7510,10 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="C118" s="0" t="s">
         <v>651</v>
@@ -7546,7 +7527,7 @@
         <v>293</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>2000</v>
+        <v>2012</v>
       </c>
       <c r="C119" s="0" t="s">
         <v>653</v>
@@ -7557,10 +7538,10 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="B120" s="0" t="n">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="C120" s="0" t="s">
         <v>655</v>
@@ -7571,10 +7552,10 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>2012</v>
+        <v>2008</v>
       </c>
       <c r="C121" s="0" t="s">
         <v>657</v>
@@ -7588,7 +7569,7 @@
         <v>303</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>2003</v>
+        <v>2013</v>
       </c>
       <c r="C122" s="0" t="s">
         <v>659</v>
@@ -7599,10 +7580,10 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>303</v>
+        <v>219</v>
       </c>
       <c r="B123" s="0" t="n">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="C123" s="0" t="s">
         <v>661</v>
@@ -7613,10 +7594,10 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>303</v>
+        <v>324</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>2013</v>
+        <v>2000</v>
       </c>
       <c r="C124" s="0" t="s">
         <v>663</v>
@@ -7627,7 +7608,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>219</v>
+        <v>324</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>2005</v>
@@ -7644,7 +7625,7 @@
         <v>324</v>
       </c>
       <c r="B126" s="0" t="n">
-        <v>2000</v>
+        <v>2010</v>
       </c>
       <c r="C126" s="0" t="s">
         <v>667</v>
@@ -7658,7 +7639,7 @@
         <v>324</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>2005</v>
+        <v>2014</v>
       </c>
       <c r="C127" s="0" t="s">
         <v>669</v>
@@ -7669,10 +7650,10 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>324</v>
+        <v>349</v>
       </c>
       <c r="B128" s="0" t="n">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="C128" s="0" t="s">
         <v>671</v>
@@ -7683,10 +7664,10 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="B129" s="0" t="n">
-        <v>2014</v>
+        <v>2005</v>
       </c>
       <c r="C129" s="0" t="s">
         <v>673</v>
@@ -7697,10 +7678,10 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="B130" s="0" t="n">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="C130" s="0" t="s">
         <v>675</v>
@@ -7714,7 +7695,7 @@
         <v>338</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>2005</v>
+        <v>2014</v>
       </c>
       <c r="C131" s="0" t="s">
         <v>677</v>
@@ -7728,7 +7709,7 @@
         <v>338</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="C132" s="0" t="s">
         <v>679</v>
@@ -7739,10 +7720,10 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B133" s="0" t="n">
-        <v>2014</v>
+        <v>2008</v>
       </c>
       <c r="C133" s="0" t="s">
         <v>681</v>
@@ -7753,10 +7734,10 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B134" s="0" t="n">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="C134" s="0" t="s">
         <v>683</v>
@@ -7767,10 +7748,10 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>333</v>
+        <v>352</v>
       </c>
       <c r="B135" s="0" t="n">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="C135" s="0" t="s">
         <v>685</v>
@@ -7781,10 +7762,10 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>333</v>
+        <v>363</v>
       </c>
       <c r="B136" s="0" t="n">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="C136" s="0" t="s">
         <v>687</v>
@@ -7795,10 +7776,10 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="B137" s="0" t="n">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="C137" s="0" t="s">
         <v>689</v>
@@ -7809,10 +7790,10 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B138" s="0" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C138" s="0" t="s">
         <v>691</v>
@@ -7823,10 +7804,10 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>368</v>
+        <v>319</v>
       </c>
       <c r="B139" s="0" t="n">
-        <v>2009</v>
+        <v>2003</v>
       </c>
       <c r="C139" s="0" t="s">
         <v>693</v>
@@ -7837,10 +7818,10 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="B140" s="0" t="n">
-        <v>2013</v>
+        <v>1999</v>
       </c>
       <c r="C140" s="0" t="s">
         <v>695</v>
@@ -7851,10 +7832,10 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>319</v>
+        <v>373</v>
       </c>
       <c r="B141" s="0" t="n">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="C141" s="0" t="s">
         <v>697</v>
@@ -7868,7 +7849,7 @@
         <v>373</v>
       </c>
       <c r="B142" s="0" t="n">
-        <v>1999</v>
+        <v>2010</v>
       </c>
       <c r="C142" s="0" t="s">
         <v>699</v>
@@ -7882,7 +7863,7 @@
         <v>373</v>
       </c>
       <c r="B143" s="0" t="n">
-        <v>2004</v>
+        <v>2015</v>
       </c>
       <c r="C143" s="0" t="s">
         <v>701</v>
@@ -7893,10 +7874,10 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="B144" s="0" t="n">
-        <v>2010</v>
+        <v>2000</v>
       </c>
       <c r="C144" s="0" t="s">
         <v>703</v>
@@ -7907,10 +7888,10 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="B145" s="0" t="n">
-        <v>2015</v>
+        <v>2006</v>
       </c>
       <c r="C145" s="0" t="s">
         <v>705</v>
@@ -7924,7 +7905,7 @@
         <v>385</v>
       </c>
       <c r="B146" s="0" t="n">
-        <v>2000</v>
+        <v>2011</v>
       </c>
       <c r="C146" s="0" t="s">
         <v>707</v>
@@ -7935,10 +7916,10 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B147" s="0" t="n">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="C147" s="0" t="s">
         <v>709</v>
@@ -7949,10 +7930,10 @@
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B148" s="0" t="n">
-        <v>2011</v>
+        <v>2002</v>
       </c>
       <c r="C148" s="0" t="s">
         <v>711</v>
@@ -7963,10 +7944,10 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="B149" s="0" t="n">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="C149" s="0" t="s">
         <v>713</v>
@@ -7977,10 +7958,10 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="B150" s="0" t="n">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="C150" s="0" t="s">
         <v>715</v>
@@ -7991,10 +7972,10 @@
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="B151" s="0" t="n">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="C151" s="0" t="s">
         <v>717</v>
@@ -8008,7 +7989,7 @@
         <v>401</v>
       </c>
       <c r="B152" s="0" t="n">
-        <v>2001</v>
+        <v>2013</v>
       </c>
       <c r="C152" s="0" t="s">
         <v>719</v>
@@ -8019,10 +8000,10 @@
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="B153" s="0" t="n">
-        <v>2007</v>
+        <v>1999</v>
       </c>
       <c r="C153" s="0" t="s">
         <v>721</v>
@@ -8033,10 +8014,10 @@
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="B154" s="0" t="n">
-        <v>2013</v>
+        <v>2005</v>
       </c>
       <c r="C154" s="0" t="s">
         <v>723</v>
@@ -8050,7 +8031,7 @@
         <v>410</v>
       </c>
       <c r="B155" s="0" t="n">
-        <v>1999</v>
+        <v>2010</v>
       </c>
       <c r="C155" s="0" t="s">
         <v>725</v>
@@ -8064,50 +8045,22 @@
         <v>410</v>
       </c>
       <c r="B156" s="0" t="n">
-        <v>2005</v>
+        <v>2015</v>
       </c>
       <c r="C156" s="0" t="s">
         <v>727</v>
       </c>
       <c r="D156" s="0" t="s">
         <v>728</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="B157" s="0" t="n">
-        <v>2010</v>
-      </c>
-      <c r="C157" s="0" t="s">
-        <v>729</v>
-      </c>
-      <c r="D157" s="0" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="B158" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="C158" s="0" t="s">
-        <v>731</v>
-      </c>
-      <c r="D158" s="0" t="s">
-        <v>732</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -8117,17 +8070,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D133"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.24609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="25.01"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8152,10 +8106,10 @@
         <v>2015</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8166,10 +8120,10 @@
         <v>2008</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8180,10 +8134,10 @@
         <v>2015</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8194,10 +8148,10 @@
         <v>2000</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8208,10 +8162,10 @@
         <v>2005</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8222,10 +8176,10 @@
         <v>2010</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8236,10 +8190,10 @@
         <v>2015</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8250,10 +8204,10 @@
         <v>2006</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8264,10 +8218,10 @@
         <v>1999</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8278,10 +8232,10 @@
         <v>2004</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8292,10 +8246,10 @@
         <v>2007</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8306,10 +8260,10 @@
         <v>2011</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8320,10 +8274,10 @@
         <v>2001</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8334,10 +8288,10 @@
         <v>2006</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8348,10 +8302,10 @@
         <v>2011</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8359,13 +8313,13 @@
         <v>43</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8376,10 +8330,10 @@
         <v>2003</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8390,10 +8344,10 @@
         <v>2008</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8404,10 +8358,10 @@
         <v>2003</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8418,10 +8372,10 @@
         <v>2010</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8432,10 +8386,10 @@
         <v>2010</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8446,10 +8400,10 @@
         <v>2017</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8460,10 +8414,10 @@
         <v>2005</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8474,10 +8428,10 @@
         <v>2010</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8488,10 +8442,10 @@
         <v>2014</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8502,10 +8456,10 @@
         <v>2004</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8516,10 +8470,10 @@
         <v>2011</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8530,10 +8484,10 @@
         <v>2004</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8544,10 +8498,10 @@
         <v>2014</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8558,10 +8512,10 @@
         <v>2015</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8572,10 +8526,10 @@
         <v>2012</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8586,10 +8540,10 @@
         <v>2005</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8600,10 +8554,10 @@
         <v>2011</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8614,10 +8568,10 @@
         <v>2011</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8628,10 +8582,10 @@
         <v>2002</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8642,10 +8596,10 @@
         <v>2007</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8656,10 +8610,10 @@
         <v>2013</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8670,10 +8624,10 @@
         <v>2007</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8684,10 +8638,10 @@
         <v>2013</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8698,10 +8652,10 @@
         <v>2000</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8712,10 +8666,10 @@
         <v>2005</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8726,10 +8680,10 @@
         <v>2011</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8740,10 +8694,10 @@
         <v>2016</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8754,10 +8708,10 @@
         <v>2000</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8768,10 +8722,10 @@
         <v>2012</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8782,10 +8736,10 @@
         <v>2013</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8796,10 +8750,10 @@
         <v>2003</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8810,10 +8764,10 @@
         <v>2008</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8824,10 +8778,10 @@
         <v>2014</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8838,10 +8792,10 @@
         <v>2014</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8852,10 +8806,10 @@
         <v>1999</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8866,10 +8820,10 @@
         <v>2005</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8880,10 +8834,10 @@
         <v>2012</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8894,10 +8848,10 @@
         <v>2009</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8908,10 +8862,10 @@
         <v>2000</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8922,10 +8876,10 @@
         <v>2005</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8936,10 +8890,10 @@
         <v>2012</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8950,10 +8904,10 @@
         <v>2011</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8964,24 +8918,24 @@
         <v>2005</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>2015</v>
+        <v>2002</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8989,13 +8943,13 @@
         <v>163</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>2002</v>
+        <v>2007</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9003,41 +8957,41 @@
         <v>163</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>2007</v>
+        <v>2012</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>163</v>
+        <v>195</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>2012</v>
+        <v>1999</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>1999</v>
+        <v>2003</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9045,13 +8999,13 @@
         <v>179</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>2003</v>
+        <v>2008</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9059,41 +9013,41 @@
         <v>179</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>2012</v>
+        <v>2004</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9101,13 +9055,13 @@
         <v>209</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>2004</v>
+        <v>2009</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9115,27 +9069,27 @@
         <v>209</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>2009</v>
+        <v>2014</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9143,27 +9097,27 @@
         <v>204</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>2013</v>
+        <v>2003</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9171,27 +9125,27 @@
         <v>222</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>2003</v>
+        <v>2008</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>2008</v>
+        <v>2000</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9199,13 +9153,13 @@
         <v>244</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>2000</v>
+        <v>2004</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9213,13 +9167,13 @@
         <v>244</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>2004</v>
+        <v>2010</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9227,41 +9181,41 @@
         <v>244</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>2009</v>
+        <v>2001</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9269,13 +9223,13 @@
         <v>227</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>2001</v>
+        <v>2006</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9283,27 +9237,27 @@
         <v>227</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>227</v>
+        <v>253</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9311,41 +9265,41 @@
         <v>253</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>2003</v>
+        <v>2011</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>236</v>
+        <v>277</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9353,13 +9307,13 @@
         <v>277</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9367,27 +9321,27 @@
         <v>277</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>2006</v>
+        <v>2013</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>2013</v>
+        <v>2001</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9395,13 +9349,13 @@
         <v>284</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>2001</v>
+        <v>2006</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9409,13 +9363,13 @@
         <v>284</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9423,27 +9377,27 @@
         <v>284</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>2016</v>
+        <v>2006</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9451,27 +9405,27 @@
         <v>272</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>2012</v>
+        <v>1999</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9479,13 +9433,13 @@
         <v>261</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>1999</v>
+        <v>2003</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9493,13 +9447,13 @@
         <v>261</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>2003</v>
+        <v>2008</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9507,13 +9461,13 @@
         <v>261</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>2008</v>
+        <v>2013</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9521,69 +9475,69 @@
         <v>261</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>2013</v>
+        <v>2018</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>261</v>
+        <v>312</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>303</v>
+        <v>219</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>2003</v>
+        <v>2005</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>219</v>
+        <v>324</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>2005</v>
+        <v>2000</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9591,13 +9545,13 @@
         <v>324</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>2000</v>
+        <v>2005</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9605,13 +9559,13 @@
         <v>324</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9619,41 +9573,41 @@
         <v>324</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>324</v>
+        <v>349</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>2014</v>
+        <v>2008</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9661,13 +9615,13 @@
         <v>338</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9675,13 +9629,13 @@
         <v>338</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9689,27 +9643,27 @@
         <v>338</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>2015</v>
+        <v>2008</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9717,69 +9671,69 @@
         <v>333</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>2008</v>
+        <v>2013</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>333</v>
+        <v>352</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>352</v>
+        <v>368</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>2009</v>
+        <v>2013</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>2013</v>
+        <v>1999</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9787,13 +9741,13 @@
         <v>373</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>1999</v>
+        <v>2004</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9801,13 +9755,13 @@
         <v>373</v>
       </c>
       <c r="B120" s="0" t="n">
-        <v>2004</v>
+        <v>2010</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9815,27 +9769,27 @@
         <v>373</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9843,13 +9797,13 @@
         <v>385</v>
       </c>
       <c r="B123" s="0" t="n">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9857,41 +9811,41 @@
         <v>385</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B125" s="0" t="n">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>382</v>
+        <v>401</v>
       </c>
       <c r="B126" s="0" t="n">
-        <v>2007</v>
+        <v>2001</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9899,13 +9853,13 @@
         <v>401</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>2001</v>
+        <v>2007</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9913,27 +9867,27 @@
         <v>401</v>
       </c>
       <c r="B128" s="0" t="n">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="B129" s="0" t="n">
-        <v>2013</v>
+        <v>1999</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9941,13 +9895,13 @@
         <v>410</v>
       </c>
       <c r="B130" s="0" t="n">
-        <v>1999</v>
+        <v>2005</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9955,13 +9909,13 @@
         <v>410</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9969,36 +9923,22 @@
         <v>410</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="B133" s="0" t="n">
-        <v>2015</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>995</v>
-      </c>
-      <c r="D133" s="0" t="s">
-        <v>996</v>
+        <v>990</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -10008,16 +9948,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.24609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.02"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10042,24 +9984,24 @@
         <v>2010</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>998</v>
+        <v>992</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>999</v>
+        <v>993</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1000</v>
+        <v>994</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10070,66 +10012,66 @@
         <v>2012</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1001</v>
+        <v>995</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1002</v>
+        <v>996</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>991</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>997</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>1003</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1004</v>
+        <v>998</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>1008</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10140,38 +10082,38 @@
         <v>2014</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>1009</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>1011</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>1013</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10182,24 +10124,24 @@
         <v>2014</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>1014</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1015</v>
+        <v>1009</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>1016</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10210,831 +10152,803 @@
         <v>2010</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>1017</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>67</v>
+        <v>1012</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>1018</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1019</v>
+        <v>72</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>1020</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>72</v>
+        <v>1015</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>1021</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1022</v>
+        <v>1015</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>1023</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1022</v>
+        <v>89</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>1024</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>1025</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>62</v>
+        <v>1020</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>1026</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1027</v>
+        <v>119</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>1028</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>119</v>
+        <v>1023</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2011</v>
+        <v>2014</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>997</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>1029</v>
+        <v>991</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>1024</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>997</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>1030</v>
+        <v>991</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>1025</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1031</v>
+        <v>1026</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1032</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>141</v>
+        <v>1028</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1034</v>
+        <v>195</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1035</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1036</v>
+        <v>195</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1037</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>195</v>
+        <v>1033</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1039</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>201</v>
+        <v>244</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>1040</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>1041</v>
+        <v>227</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1042</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>1043</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>227</v>
+        <v>1038</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1044</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>227</v>
+        <v>1038</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1045</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>1046</v>
+        <v>1041</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>1047</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>1049</v>
+        <v>1043</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1050</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>1051</v>
+        <v>1046</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>1052</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>1051</v>
+        <v>284</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>1053</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>1054</v>
+        <v>261</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1056</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>261</v>
+        <v>1051</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1057</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>261</v>
+        <v>1051</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>1058</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>1059</v>
+        <v>1054</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>1060</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>1062</v>
+        <v>219</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1063</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>1064</v>
+        <v>1059</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1065</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>219</v>
+        <v>349</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>1066</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>1067</v>
+        <v>1062</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>1068</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>349</v>
+        <v>1062</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1069</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>1070</v>
+        <v>333</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>1071</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1072</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>333</v>
+        <v>1068</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>1074</v>
+        <v>1068</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>1075</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>1076</v>
+        <v>1071</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>1077</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>1076</v>
+        <v>352</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1078</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>1079</v>
+        <v>352</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>1080</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>352</v>
+        <v>1075</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>1081</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>352</v>
+        <v>1077</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>1083</v>
+        <v>1077</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>1084</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>1085</v>
+        <v>360</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>1086</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>1087</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>360</v>
+        <v>1083</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>1091</v>
+        <v>382</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>1092</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>1093</v>
+        <v>1088</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1094</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>1095</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>1096</v>
+        <v>392</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>392</v>
+        <v>410</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>392</v>
-      </c>
-      <c r="B71" s="0" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>997</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="B72" s="0" t="n">
-        <v>2014</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>997</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>1100</v>
+        <v>1092</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update auxiliary data. fix bugs
</commit_message>
<xml_diff>
--- a/auxiliary_data/filenames.xlsx
+++ b/auxiliary_data/filenames.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="dhs_pr_files" sheetId="1" state="visible" r:id="rId2"/>
@@ -3010,7 +3010,7 @@
     <t xml:space="preserve">Algeria/2012/hl.dta</t>
   </si>
   <si>
-    <t xml:space="preserve">Bangladesh/2012/hl.dta</t>
+    <t xml:space="preserve">Bangladesh/2013/hl.dta</t>
   </si>
   <si>
     <t xml:space="preserve">Barbados</t>
@@ -3387,12 +3387,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -3404,17 +3404,16 @@
   </sheetPr>
   <dimension ref="A1:D173"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="65.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="65.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5842,10 +5841,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5857,17 +5856,15 @@
   </sheetPr>
   <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.9540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8057,10 +8054,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -8072,16 +8069,15 @@
   </sheetPr>
   <dimension ref="A1:D132"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="21.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9935,10 +9931,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -9950,16 +9946,14 @@
   </sheetPr>
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10009,7 +10003,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>991</v>
@@ -10945,10 +10939,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>